<commit_message>
updated extractor unit tests to test for trailing white spaces in headers
</commit_message>
<xml_diff>
--- a/test/mock/excel_mock.xlsx
+++ b/test/mock/excel_mock.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>One</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Three Things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trailing spaces   </t>
   </si>
 </sst>
 </file>
@@ -362,15 +365,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,8 +383,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -391,8 +397,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -401,6 +410,9 @@
       </c>
       <c r="C3" t="s">
         <v>5</v>
+      </c>
+      <c r="D3">
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>